<commit_message>
update diagram and flow
</commit_message>
<xml_diff>
--- a/Reference Architecture - for publishing artefacts.xlsx
+++ b/Reference Architecture - for publishing artefacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estani002\Documents\GitHub\reference-architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917D424-4E22-426E-9ADF-B0990CBD9B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DB952C-B918-4C4E-B070-77F4C70E5B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,14 +547,11 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -567,6 +564,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,8 +788,8 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -801,17 +801,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -827,7 +827,7 @@
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -855,7 +855,7 @@
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -907,7 +907,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -946,7 +946,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1003,7 +1003,7 @@
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1042,7 +1042,7 @@
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1123,7 +1123,7 @@
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1149,7 +1149,7 @@
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="24" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -1208,7 +1208,7 @@
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B34" s="3" t="s">

</xml_diff>